<commit_message>
Made up controls for example 2
</commit_message>
<xml_diff>
--- a/Cyclo_noncyclo_comparison/Examples/Example2/Inputs/madeup_positive_controls.xlsx
+++ b/Cyclo_noncyclo_comparison/Examples/Example2/Inputs/madeup_positive_controls.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hank\Documents\Research\Projects\Iso-seq_public\Cyclo_noncyclo_comparison\Examples\Example2\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5185CB72-18F0-4D90-9E97-25A832000B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7536AE-70E2-4075-B8C2-726B816265A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="2" xr2:uid="{B63E0232-D77F-4A71-81C7-BBF627DB2C1D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{B63E0232-D77F-4A71-81C7-BBF627DB2C1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,17 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>Hyp1</t>
   </si>
   <si>
-    <t>Hyp2</t>
-  </si>
-  <si>
-    <t>Hyp3</t>
-  </si>
-  <si>
     <t>Hyp5</t>
   </si>
   <si>
@@ -58,9 +51,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Above/below median</t>
-  </si>
-  <si>
     <t>PB.1</t>
   </si>
   <si>
@@ -73,25 +63,10 @@
     <t>PB.5</t>
   </si>
   <si>
-    <t>PB.1, Gene1</t>
-  </si>
-  <si>
-    <t>PB.2, Gene2</t>
-  </si>
-  <si>
     <t>GeneB</t>
   </si>
   <si>
     <t>GeneA</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Above</t>
-  </si>
-  <si>
-    <t>PB.3, Gene3</t>
   </si>
   <si>
     <t>GeneC</t>
@@ -678,94 +653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66E72E1-897C-41E5-A60F-E57C9169D14E}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFCBB26-0AD6-4E71-9ACB-E85936D88997}">
   <dimension ref="A2:K34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,28 +673,28 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -812,390 +704,390 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="F16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
         <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1204,11 +1096,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486AF542-DBFA-4B1A-8BC6-E9C5CB8E5113}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -1216,33 +1108,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>70</v>
@@ -1271,7 +1163,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1300,7 +1192,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -1329,7 +1221,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1358,7 +1250,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1387,7 +1279,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -1416,7 +1308,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -1445,7 +1337,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -1474,7 +1366,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -1503,7 +1395,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1532,7 +1424,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1561,7 +1453,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1590,7 +1482,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1619,7 +1511,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1648,7 +1540,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -1677,7 +1569,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>1000</v>
@@ -1706,7 +1598,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B18">
         <v>30</v>

</xml_diff>